<commit_message>
updated excel - person column
</commit_message>
<xml_diff>
--- a/sadna_nevo_and_ofir.xlsx
+++ b/sadna_nevo_and_ofir.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ofirkatz/Docs2019/School/year4/semesterA/sadna/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C363D4-E015-2249-88B2-18376A79ADD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E426DA-436F-E84E-AFE4-69BF04FD2473}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="13840" xr2:uid="{E1C877FC-E5CA-7249-B453-02312586D4B7}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
   <si>
     <t>Category</t>
   </si>
@@ -205,13 +205,22 @@
   </si>
   <si>
     <t>https://www.analyticsvidhya.com/blog/2019/10/gaussian-mixture-models-clustering/</t>
+  </si>
+  <si>
+    <t>person</t>
+  </si>
+  <si>
+    <t>nevo</t>
+  </si>
+  <si>
+    <t>ofir</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -231,6 +240,13 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -278,7 +294,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -286,6 +302,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -601,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C25CD2B-D3C4-EF48-ADEA-1A53DB30F24A}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -612,14 +630,15 @@
     <col min="1" max="1" width="36.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -628,13 +647,16 @@
         <v>17</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -644,14 +666,14 @@
       <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -661,14 +683,14 @@
       <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -678,14 +700,14 @@
       <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -695,14 +717,14 @@
       <c r="C6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -712,14 +734,14 @@
       <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -729,45 +751,51 @@
       <c r="C8" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="F10" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
@@ -777,39 +805,45 @@
       <c r="C11" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="F12" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
@@ -819,14 +853,14 @@
       <c r="C14" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="F14" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
@@ -836,10 +870,10 @@
       <c r="C15" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="F15" s="5" t="s">
         <v>46</v>
       </c>
     </row>
@@ -855,31 +889,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{AFA00709-6D62-B245-BC7A-98F5A3CDD0FC}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{62F3EDAE-458F-2A4A-95EF-5E3E5165C970}"/>
-    <hyperlink ref="D5" r:id="rId3" xr:uid="{DF5860D6-FDEF-2748-A850-355F5EE920B2}"/>
-    <hyperlink ref="D6" r:id="rId4" xr:uid="{7AC54448-E1C2-E747-995E-DDF0443D8AAE}"/>
-    <hyperlink ref="D7" r:id="rId5" xr:uid="{CDCC8BC4-89D6-F741-A678-548ACA40DF73}"/>
-    <hyperlink ref="D8" r:id="rId6" xr:uid="{307A8FA0-290B-F546-8C13-891BCC83DB7E}"/>
-    <hyperlink ref="D9" r:id="rId7" xr:uid="{50C1FAB4-8BED-4549-8C4A-DCC6E63C33D0}"/>
-    <hyperlink ref="D10" r:id="rId8" xr:uid="{D2D30950-5625-3246-9F85-71C12E1FDC66}"/>
-    <hyperlink ref="D11" r:id="rId9" xr:uid="{31DD3F90-C398-F24C-AD05-2879D0F271DB}"/>
-    <hyperlink ref="D12" r:id="rId10" xr:uid="{C7846971-7459-7242-9111-051765C6DE51}"/>
-    <hyperlink ref="E13" r:id="rId11" xr:uid="{B9A4639F-B65D-A746-AC6C-B1FE56C009E7}"/>
-    <hyperlink ref="D14" r:id="rId12" xr:uid="{C3A63692-A10F-7645-BF93-EF45E679F3D1}"/>
-    <hyperlink ref="D15" r:id="rId13" xr:uid="{6A4E6A44-D1E4-574C-8D31-6BE0F1178017}"/>
-    <hyperlink ref="E15" r:id="rId14" xr:uid="{D15D89C4-5069-9149-82B2-6A0E24D1F3FB}"/>
-    <hyperlink ref="E14" r:id="rId15" xr:uid="{03AD3697-6266-BE4F-A291-ADE217C6499C}"/>
-    <hyperlink ref="E3" r:id="rId16" xr:uid="{BE6E1969-68B9-1B4E-ADEA-701F5B7ED5FC}"/>
-    <hyperlink ref="E4" r:id="rId17" xr:uid="{F0C84C6C-017C-7A4F-BE81-EEAA5E39FBA7}"/>
-    <hyperlink ref="E5" r:id="rId18" xr:uid="{4FC7A365-7D0F-554F-8717-002D7A551E1F}"/>
-    <hyperlink ref="E6" r:id="rId19" xr:uid="{FFBC508A-2703-8F4C-BE81-E301C702FD2A}"/>
-    <hyperlink ref="E7" r:id="rId20" xr:uid="{7D7847C2-5C55-524A-95E7-77E9277C05E5}"/>
-    <hyperlink ref="E8" r:id="rId21" xr:uid="{0CED3320-1E41-3A47-B760-8205254E444B}"/>
-    <hyperlink ref="E9" r:id="rId22" xr:uid="{74C0F30E-B965-DF4A-BCD0-383DBE7CDB09}"/>
-    <hyperlink ref="E10" r:id="rId23" xr:uid="{07118DD1-B904-DD46-85F9-17A857BDD511}"/>
-    <hyperlink ref="E11" r:id="rId24" xr:uid="{89C8D544-33FE-C041-BBE7-C1B26C970FB0}"/>
-    <hyperlink ref="E12" r:id="rId25" xr:uid="{95594A6E-34AE-DB42-939B-1FE203A86171}"/>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{AFA00709-6D62-B245-BC7A-98F5A3CDD0FC}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{62F3EDAE-458F-2A4A-95EF-5E3E5165C970}"/>
+    <hyperlink ref="E5" r:id="rId3" xr:uid="{DF5860D6-FDEF-2748-A850-355F5EE920B2}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{7AC54448-E1C2-E747-995E-DDF0443D8AAE}"/>
+    <hyperlink ref="E7" r:id="rId5" xr:uid="{CDCC8BC4-89D6-F741-A678-548ACA40DF73}"/>
+    <hyperlink ref="E8" r:id="rId6" xr:uid="{307A8FA0-290B-F546-8C13-891BCC83DB7E}"/>
+    <hyperlink ref="E9" r:id="rId7" xr:uid="{50C1FAB4-8BED-4549-8C4A-DCC6E63C33D0}"/>
+    <hyperlink ref="E10" r:id="rId8" xr:uid="{D2D30950-5625-3246-9F85-71C12E1FDC66}"/>
+    <hyperlink ref="E11" r:id="rId9" xr:uid="{31DD3F90-C398-F24C-AD05-2879D0F271DB}"/>
+    <hyperlink ref="E12" r:id="rId10" xr:uid="{C7846971-7459-7242-9111-051765C6DE51}"/>
+    <hyperlink ref="F13" r:id="rId11" xr:uid="{B9A4639F-B65D-A746-AC6C-B1FE56C009E7}"/>
+    <hyperlink ref="E14" r:id="rId12" xr:uid="{C3A63692-A10F-7645-BF93-EF45E679F3D1}"/>
+    <hyperlink ref="E15" r:id="rId13" xr:uid="{6A4E6A44-D1E4-574C-8D31-6BE0F1178017}"/>
+    <hyperlink ref="F15" r:id="rId14" xr:uid="{D15D89C4-5069-9149-82B2-6A0E24D1F3FB}"/>
+    <hyperlink ref="F14" r:id="rId15" xr:uid="{03AD3697-6266-BE4F-A291-ADE217C6499C}"/>
+    <hyperlink ref="F3" r:id="rId16" xr:uid="{BE6E1969-68B9-1B4E-ADEA-701F5B7ED5FC}"/>
+    <hyperlink ref="F4" r:id="rId17" xr:uid="{F0C84C6C-017C-7A4F-BE81-EEAA5E39FBA7}"/>
+    <hyperlink ref="F5" r:id="rId18" xr:uid="{4FC7A365-7D0F-554F-8717-002D7A551E1F}"/>
+    <hyperlink ref="F6" r:id="rId19" xr:uid="{FFBC508A-2703-8F4C-BE81-E301C702FD2A}"/>
+    <hyperlink ref="F7" r:id="rId20" xr:uid="{7D7847C2-5C55-524A-95E7-77E9277C05E5}"/>
+    <hyperlink ref="F8" r:id="rId21" xr:uid="{0CED3320-1E41-3A47-B760-8205254E444B}"/>
+    <hyperlink ref="F9" r:id="rId22" xr:uid="{74C0F30E-B965-DF4A-BCD0-383DBE7CDB09}"/>
+    <hyperlink ref="F10" r:id="rId23" xr:uid="{07118DD1-B904-DD46-85F9-17A857BDD511}"/>
+    <hyperlink ref="F11" r:id="rId24" xr:uid="{89C8D544-33FE-C041-BBE7-C1B26C970FB0}"/>
+    <hyperlink ref="F12" r:id="rId25" xr:uid="{95594A6E-34AE-DB42-939B-1FE203A86171}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>